<commit_message>
create size column in student
</commit_message>
<xml_diff>
--- a/WebApplication1/importexcel.xlsx
+++ b/WebApplication1/importexcel.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>address</t>
   </si>
@@ -31,21 +31,6 @@
   </si>
   <si>
     <t>photo</t>
-  </si>
-  <si>
-    <t>lko</t>
-  </si>
-  <si>
-    <t>abc</t>
-  </si>
-  <si>
-    <t>test5</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>images.jpeg</t>
   </si>
   <si>
     <t>rollno</t>
@@ -131,7 +116,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -433,118 +418,87 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U2"/>
+  <dimension ref="A1:U1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U2" sqref="U2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="13.7109375" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="21.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G1" t="s">
         <v>2</v>
       </c>
       <c r="H1" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="I1" t="s">
         <v>3</v>
       </c>
       <c r="J1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="K1" t="s">
         <v>4</v>
       </c>
       <c r="L1" t="s">
+        <v>5</v>
+      </c>
+      <c r="M1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N1" t="s">
+        <v>8</v>
+      </c>
+      <c r="O1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P1" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
+      <c r="R1" t="s">
+        <v>11</v>
+      </c>
+      <c r="S1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" t="s">
-        <v>16</v>
-      </c>
-      <c r="S1" t="s">
-        <v>17</v>
-      </c>
       <c r="T1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="U1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="1">
-        <v>44925</v>
-      </c>
-      <c r="G2">
-        <v>12345</v>
-      </c>
-      <c r="I2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J2" t="s">
-        <v>8</v>
-      </c>
-      <c r="K2" t="s">
-        <v>9</v>
-      </c>
-      <c r="L2">
-        <v>2</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>